<commit_message>
aktualizcja przebiegu imprezy, kosztów, nr konta
</commit_message>
<xml_diff>
--- a/Kawalerski Marcina Details.xlsx
+++ b/Kawalerski Marcina Details.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Michal\OneDrive\Projekty\Kawalerskie Marcina\KawalerskiMarcina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4FC30-EE5E-4221-A01A-FBBFBABC9C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9935971-5414-4D8C-B90F-911EA90A2B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A88B5DC-3333-4EF2-BEF8-D9380C72974E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7A88B5DC-3333-4EF2-BEF8-D9380C72974E}"/>
   </bookViews>
   <sheets>
     <sheet name="Przebieg Imprezy" sheetId="1" r:id="rId1"/>
-    <sheet name="Miejsca" sheetId="4" r:id="rId2"/>
-    <sheet name="Budget" sheetId="2" r:id="rId3"/>
-    <sheet name="Lista osób" sheetId="3" r:id="rId4"/>
+    <sheet name="Budget" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista osób + wpłaty" sheetId="3" r:id="rId3"/>
+    <sheet name="Miejsca" sheetId="4" r:id="rId4"/>
+    <sheet name="Nr Konta do wpłaty" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>Pomysły</t>
   </si>
@@ -78,9 +79,6 @@
     </r>
   </si>
   <si>
-    <t>Przyjazd Marcina w umówione miejsce</t>
-  </si>
-  <si>
     <t>Forma</t>
   </si>
   <si>
@@ -111,9 +109,6 @@
     <t>16:30 - 18:30</t>
   </si>
   <si>
-    <t>Dojazd do party housa</t>
-  </si>
-  <si>
     <t>Marcin</t>
   </si>
   <si>
@@ -219,9 +214,6 @@
     <t>Koszty Na os</t>
   </si>
   <si>
-    <t>Czterech ziomków odbiera go furą, musi rozwiązać zadanie aby znaleźć pierwsze miejsce. Dojazd do pierwszego miejsca. Bez alko póki co</t>
-  </si>
-  <si>
     <t>Pierwsze miejsce Gokarty- Marcin 2x przejazdy, 2x grupy przeciwników każda osobny przejazd , rozwiązanie zagadki</t>
   </si>
   <si>
@@ -237,9 +229,6 @@
     <t>19:00 - 20:00</t>
   </si>
   <si>
-    <t>Trzecie miejsce - house szkolna, Marcin dostanie od barmana instrukcje do rozwiązania gdzie jest party house. Kilka szotów dla każdego na miejscu.</t>
-  </si>
-  <si>
     <t>Przebieg imprezy Dzień 2 (DLA CHĘTNYCH):</t>
   </si>
   <si>
@@ -261,9 +250,6 @@
     <t>Dzień 2</t>
   </si>
   <si>
-    <t>18 dołków</t>
-  </si>
-  <si>
     <t>Koszyk Piłek</t>
   </si>
   <si>
@@ -285,9 +271,6 @@
     <t>www</t>
   </si>
   <si>
-    <t>Afterek w mieszkaniu u drużby (ograniczona liczba miejsc do spania)</t>
-  </si>
-  <si>
     <t>Golf</t>
   </si>
   <si>
@@ -343,6 +326,54 @@
   </si>
   <si>
     <t>Background: Marcin będzie musiał rozwiązywac zagadki aby dotrzeć do każdego miejsca i wykonać zadania. Reszta ekipy będzie podzielona na dwie grupy. Bedąc w kominiarkach, lub nie, na zmianę będą mu przeszkadzać w wykonaniu zadania, tj. Uderzać go na gokartach, być w przeciwnej drużynie w laser tagach. Po każdym wykonanym zadaniu będzie dostawał następne instrukcje. Ostateczny punkt to Party House.</t>
+  </si>
+  <si>
+    <t>Wpłata</t>
+  </si>
+  <si>
+    <t>+48 693 111 274</t>
+  </si>
+  <si>
+    <t>House Club</t>
+  </si>
+  <si>
+    <t>9 dołków</t>
+  </si>
+  <si>
+    <t>Przyjazd Marcina w umówione miejsce ze świadkiem</t>
+  </si>
+  <si>
+    <t>Marcin rozwiązuje zagadkę i dociera uberem albo komunikacją miejską do gokartów. Tam będzie zebranie wszystkich. Bez alko póki co</t>
+  </si>
+  <si>
+    <t>Koniec kawalerskiego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trzecie miejsce - house szkolna, Marcin dostanie od barmana instrukcje do rozwiązania gdzie jest party house. Kilka szotów dla każdego na miejscu. Open bar na 800 zł. </t>
+  </si>
+  <si>
+    <t>Dojazd do party housa. Na Marcina będzie czekał prezent. Pizza lub catering na miejscu.</t>
+  </si>
+  <si>
+    <t>Odbiorca</t>
+  </si>
+  <si>
+    <t>Nr Konta</t>
+  </si>
+  <si>
+    <t>Tytuł</t>
+  </si>
+  <si>
+    <t>Imię i nazwisko lub numer telefonu do identyfikacji</t>
+  </si>
+  <si>
+    <t>42 1140 2004 0000 3902 5514 5929</t>
+  </si>
+  <si>
+    <t>Michal Warakomski</t>
+  </si>
+  <si>
+    <t>Opłacono</t>
   </si>
 </sst>
 </file>
@@ -352,7 +383,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +423,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -524,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
@@ -597,7 +634,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -915,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD1BA5-DE24-406D-A141-5E5F3B51E8A1}">
   <dimension ref="A2:D25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -964,7 +1002,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="15"/>
       <c r="C7" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -973,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -982,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -991,10 +1029,10 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -1002,7 +1040,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2"/>
     </row>
@@ -1011,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="D13" s="8">
         <v>0.58333333333333337</v>
@@ -1022,10 +1060,10 @@
         <v>2</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1033,10 +1071,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1044,10 +1082,10 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -1055,10 +1093,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -1066,10 +1104,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1077,10 +1115,10 @@
         <v>7</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -1088,7 +1126,7 @@
         <v>8</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="D20" s="8">
         <v>0.875</v>
@@ -1097,10 +1135,10 @@
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="C22" s="29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -1108,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1117,10 +1155,10 @@
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -1128,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="D25" s="8">
         <v>0.75</v>
@@ -1141,11 +1179,607 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7767389B-2498-4A1B-A331-98FBA0E9F43B}">
+  <dimension ref="B2:P12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="13.88671875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="3">
+        <v>80</v>
+      </c>
+      <c r="H3" s="3">
+        <v>75</v>
+      </c>
+      <c r="I3" s="3">
+        <v>75</v>
+      </c>
+      <c r="J3" s="3">
+        <f>J5/(C$4+1)</f>
+        <v>125</v>
+      </c>
+      <c r="K3" s="3">
+        <v>100</v>
+      </c>
+      <c r="L3" s="3">
+        <v>25</v>
+      </c>
+      <c r="M3" s="3">
+        <v>50</v>
+      </c>
+      <c r="N3" s="3">
+        <f>SUM(G3:M3)</f>
+        <v>530</v>
+      </c>
+      <c r="O3" s="3">
+        <f>N3*$C$4</f>
+        <v>7950</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="3">
+        <f>ROUNDUP(N5,-1)</f>
+        <v>570</v>
+      </c>
+      <c r="C4" s="2">
+        <f>'Lista osób + wpłaty'!C19</f>
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <f>B4*C4+'Lista osób + wpłaty'!E3</f>
+        <v>9550</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3">
+        <v>145</v>
+      </c>
+      <c r="H4" s="3">
+        <v>75</v>
+      </c>
+      <c r="I4" s="3">
+        <v>75</v>
+      </c>
+      <c r="J4" s="3">
+        <f>J5/(C$4+1)</f>
+        <v>125</v>
+      </c>
+      <c r="K4" s="3">
+        <v>100</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3">
+        <v>50</v>
+      </c>
+      <c r="N4" s="3">
+        <f>SUM(G4:M4)/$C$4</f>
+        <v>38</v>
+      </c>
+      <c r="O4" s="3">
+        <f>SUM(G4:M4)</f>
+        <v>570</v>
+      </c>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F5" s="32" t="str">
+        <f>"Total x"&amp;$C$4&amp;""</f>
+        <v>Total x15</v>
+      </c>
+      <c r="G5" s="3">
+        <f>(G3*$C$4)+G4</f>
+        <v>1345</v>
+      </c>
+      <c r="H5" s="3">
+        <f>(H3*$C$4)+H4</f>
+        <v>1200</v>
+      </c>
+      <c r="I5" s="3">
+        <f>(I3*$C$4)+I4</f>
+        <v>1200</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="3">
+        <f>(K3*$C$4)+K4</f>
+        <v>1600</v>
+      </c>
+      <c r="L5" s="3">
+        <f>(L3*$C$4)+L4+'Lista osób + wpłaty'!E3</f>
+        <v>1375</v>
+      </c>
+      <c r="M5" s="3">
+        <f>(M3*$C$4)+M4</f>
+        <v>800</v>
+      </c>
+      <c r="N5" s="22">
+        <f>SUM(N3:N4)</f>
+        <v>568</v>
+      </c>
+      <c r="O5" s="22">
+        <f>SUM(G5:M5)</f>
+        <v>9520</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F6" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="3">
+        <v>230</v>
+      </c>
+      <c r="H9" s="3">
+        <v>25</v>
+      </c>
+      <c r="I9" s="3">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3">
+        <v>150</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
+        <f>SUM(G9:M9)</f>
+        <v>415</v>
+      </c>
+      <c r="O9" s="3">
+        <f>N9*$C$10</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="3">
+        <f>ROUNDUP(N11,-1)</f>
+        <v>440</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3">
+        <v>230</v>
+      </c>
+      <c r="H10" s="3">
+        <v>25</v>
+      </c>
+      <c r="I10" s="3">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3">
+        <f>SUM(G10:M10)/$C$4</f>
+        <v>17.666666666666668</v>
+      </c>
+      <c r="O10" s="3">
+        <f>SUM(G10:M10)</f>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F11" s="13" t="str">
+        <f>"Total x"&amp;$C$4&amp;""</f>
+        <v>Total x15</v>
+      </c>
+      <c r="G11" s="3">
+        <f>(G9*$C$10)+G10</f>
+        <v>460</v>
+      </c>
+      <c r="H11" s="3">
+        <f>SUM(H9:H10)</f>
+        <v>50</v>
+      </c>
+      <c r="I11" s="3">
+        <f>SUM(I9:I10)</f>
+        <v>20</v>
+      </c>
+      <c r="J11" s="3">
+        <f>SUM(J9:J10)</f>
+        <v>150</v>
+      </c>
+      <c r="K11" s="3">
+        <f>(K9*$C$4)+K10</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <f>(L9*$C$4)+L10</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
+        <f>(M9*$C$4)+M10</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="22">
+        <f>SUM(N9:N10)</f>
+        <v>432.66666666666669</v>
+      </c>
+      <c r="O11" s="22">
+        <f>SUM(G11:M11)</f>
+        <v>680</v>
+      </c>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="N12" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494CA11B-2E48-4329-BE28-A63E56EE80BE}">
+  <dimension ref="B2:E19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="12">
+        <v>13</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
+        <v>14</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
+        <v>15</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
+        <v>16</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="20">
+        <f>COUNTIF(D3:D18,TRUE)-1</f>
+        <v>15</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D247EB18-DE83-457C-8655-07698304A578}">
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1154,25 +1788,25 @@
     <col min="4" max="4" width="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65.44140625" customWidth="1"/>
     <col min="6" max="6" width="14.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="11"/>
       <c r="C2" s="23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -1180,17 +1814,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="35"/>
+        <v>77</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>88</v>
+      </c>
       <c r="G3" s="34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -1198,19 +1834,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>88</v>
-      </c>
       <c r="G4" s="34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -1218,17 +1854,17 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F5" s="35"/>
       <c r="G5" s="34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -1236,17 +1872,17 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="33" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -1254,19 +1890,19 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E7" s="33" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F7" s="35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1287,543 +1923,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7767389B-2498-4A1B-A331-98FBA0E9F43B}">
-  <dimension ref="B2:P11"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2420CD1D-5D03-4853-A06F-D4D308B6F168}">
+  <dimension ref="B2:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.109375" style="4"/>
-    <col min="9" max="12" width="13.88671875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="4"/>
-    <col min="14" max="14" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="4"/>
+    <col min="3" max="3" width="42.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="3">
-        <v>60</v>
-      </c>
-      <c r="H3" s="3">
-        <v>75</v>
-      </c>
-      <c r="I3" s="3">
-        <v>75</v>
-      </c>
-      <c r="J3" s="3">
-        <f>J5/(C$4+1)</f>
-        <v>68.75</v>
-      </c>
-      <c r="K3" s="3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="18"/>
+      <c r="C2" s="26"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3">
-        <f>SUM(G3:M3)</f>
-        <v>378.75</v>
-      </c>
-      <c r="O3" s="3">
-        <f>N3*$C$4</f>
-        <v>5681.25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>500</v>
-      </c>
-      <c r="C4" s="2">
-        <f>'Lista osób'!C19</f>
-        <v>15</v>
-      </c>
-      <c r="D4" s="2">
-        <f>B4*C4</f>
-        <v>7500</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3">
-        <v>120</v>
-      </c>
-      <c r="H4" s="3">
-        <v>75</v>
-      </c>
-      <c r="I4" s="3">
-        <v>75</v>
-      </c>
-      <c r="J4" s="3">
-        <f>J5/(C$4+1)</f>
-        <v>68.75</v>
-      </c>
-      <c r="K4" s="3">
-        <v>100</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3">
-        <f>SUM(G4:M4)/$C$4</f>
-        <v>29.25</v>
-      </c>
-      <c r="O4" s="3">
-        <f>SUM(G4:M4)</f>
-        <v>438.75</v>
-      </c>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F5" s="13" t="str">
-        <f>"Total x"&amp;$C$4&amp;""</f>
-        <v>Total x15</v>
-      </c>
-      <c r="G5" s="3">
-        <f>(G3*$C$4)+G4</f>
-        <v>1020</v>
-      </c>
-      <c r="H5" s="3">
-        <f>(H3*$C$4)+H4</f>
-        <v>1200</v>
-      </c>
-      <c r="I5" s="3">
-        <f>(I3*$C$4)+I4</f>
-        <v>1200</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1100</v>
-      </c>
-      <c r="K5" s="3">
-        <f>(K3*$C$4)+K4</f>
-        <v>1600</v>
-      </c>
-      <c r="L5" s="3">
-        <f>(L3*$C$4)+L4</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="3">
-        <f>(M3*$C$4)+M4</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="22">
-        <f>SUM(N3:N4)</f>
-        <v>408</v>
-      </c>
-      <c r="O5" s="22">
-        <f>SUM(G5:M5)</f>
-        <v>6120</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="3">
-        <v>290</v>
-      </c>
-      <c r="H8" s="3">
-        <v>25</v>
-      </c>
-      <c r="I8" s="3">
-        <v>10</v>
-      </c>
-      <c r="J8" s="3">
-        <v>150</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3">
-        <f>SUM(G8:M8)</f>
-        <v>475</v>
-      </c>
-      <c r="O8" s="3">
-        <f>N8*$B$9</f>
-        <v>475</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3">
-        <v>290</v>
-      </c>
-      <c r="H9" s="3">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3">
-        <v>10</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3">
-        <f>SUM(G9:M9)/$C$4</f>
-        <v>21.666666666666668</v>
-      </c>
-      <c r="O9" s="3">
-        <f>SUM(G9:M9)</f>
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F10" s="13" t="str">
-        <f>"Total x"&amp;$C$4&amp;""</f>
-        <v>Total x15</v>
-      </c>
-      <c r="G10" s="3">
-        <f>(G8*$B$9)+G9</f>
-        <v>580</v>
-      </c>
-      <c r="H10" s="3">
-        <f>SUM(H8:H9)</f>
-        <v>50</v>
-      </c>
-      <c r="I10" s="3">
-        <f>SUM(I8:I9)</f>
-        <v>20</v>
-      </c>
-      <c r="J10" s="3">
-        <f>SUM(J8:J9)</f>
-        <v>150</v>
-      </c>
-      <c r="K10" s="3">
-        <f>(K8*$C$4)+K9</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="3">
-        <f>(L8*$C$4)+L9</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="3">
-        <f>(M8*$C$4)+M9</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="22">
-        <f>SUM(N8:N9)</f>
-        <v>496.66666666666669</v>
-      </c>
-      <c r="O10" s="22">
-        <f>SUM(G10:M10)</f>
-        <v>800</v>
-      </c>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="N11" s="30"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494CA11B-2E48-4329-BE28-A63E56EE80BE}">
-  <dimension ref="B2:D19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="12">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
-        <v>3</v>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="37" t="s">
+        <v>98</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="12">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="12">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="12">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="12">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="12">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="12">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="12">
-        <v>10</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="12">
-        <v>11</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="12">
-        <v>12</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="12">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="12">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="12">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="12">
-        <v>16</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" s="20">
-        <f>COUNTIF(D3:D18,TRUE)-1</f>
-        <v>15</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>